<commit_message>
Reservacion y Check In listo
</commit_message>
<xml_diff>
--- a/backend/database/seeders/Catalogos/Departamentos.xlsx
+++ b/backend/database/seeders/Catalogos/Departamentos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\SistemaMRM\database\seeds\Catalogos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hotel_restuarante\backend\database\seeders\Catalogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>Guatemala</t>
   </si>
@@ -90,6 +90,138 @@
   </si>
   <si>
     <t>Jutiapa</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>030</t>
+  </si>
+  <si>
+    <t>040</t>
+  </si>
+  <si>
+    <t>050</t>
+  </si>
+  <si>
+    <t>060</t>
+  </si>
+  <si>
+    <t>070</t>
+  </si>
+  <si>
+    <t>080</t>
+  </si>
+  <si>
+    <t>090</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
 </sst>
 </file>
@@ -125,8 +257,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,191 +540,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>